<commit_message>
added row number for graphing
</commit_message>
<xml_diff>
--- a/Data Analysis/input_parameters.xlsx
+++ b/Data Analysis/input_parameters.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Temporal Stimulation Migration Rework\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0284359-D079-4202-9A93-2462D705013A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="5490" yWindow="1125" windowWidth="18600" windowHeight="9495" xr2:uid="{DD70F028-D190-43D7-8397-96D62A5D569E}"/>
+    <workbookView xWindow="5490" yWindow="1125" windowWidth="18600" windowHeight="9495"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>food_conc</t>
   </si>
@@ -43,11 +37,14 @@
   <si>
     <t>Vo_max</t>
   </si>
+  <si>
+    <t>Row Number</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -139,7 +136,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -191,7 +188,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -385,17 +382,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BB13655-5CC4-4CF7-BC52-23F97BD2CEC3}">
-  <dimension ref="A1:E102"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F102" sqref="F2:F102"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -404,9 +403,10 @@
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -422,8 +422,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.21163331273677241</v>
       </c>
@@ -439,8 +442,12 @@
       <c r="E2">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <f>ROW(F2) - 1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.23994389380181111</v>
       </c>
@@ -456,8 +463,12 @@
       <c r="E3">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <f t="shared" ref="F3:F66" si="0">ROW(F3) - 1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.27204163384421276</v>
       </c>
@@ -473,8 +484,12 @@
       <c r="E4">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.30843314814986184</v>
       </c>
@@ -490,8 +505,12 @@
       <c r="E5">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.34969282287178255</v>
       </c>
@@ -507,8 +526,12 @@
       <c r="E6">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.3964718808648281</v>
       </c>
@@ -524,8 +547,12 @@
       <c r="E7">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.44950866027390363</v>
       </c>
@@ -541,8 +568,12 @@
       <c r="E8">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.50964026810801422</v>
       </c>
@@ -558,8 +589,12 @@
       <c r="E9">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.57781579273454453</v>
       </c>
@@ -575,8 +610,12 @@
       <c r="E10">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.65511128383342077</v>
       </c>
@@ -592,8 +631,12 @@
       <c r="E11">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.74274673624754861</v>
       </c>
@@ -609,8 +652,12 @@
       <c r="E12">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.84210534579444485</v>
       </c>
@@ -626,8 +673,12 @@
       <c r="E13">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0.95475534096353565</v>
       </c>
@@ -643,8 +694,12 @@
       <c r="E14">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1.0824747350801229</v>
       </c>
@@ -660,8 +715,12 @@
       <c r="E15">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1.2272793896122698</v>
       </c>
@@ -677,8 +736,12 @@
       <c r="E16">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1.3914548315583348</v>
       </c>
@@ -694,8 +757,12 @@
       <c r="E17">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1.5775923271054964</v>
       </c>
@@ -711,8 +778,12 @@
       <c r="E18">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1.7886297809285348</v>
       </c>
@@ -728,8 +799,12 @@
       <c r="E19">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2.0278981066637263</v>
       </c>
@@ -745,8 +820,12 @@
       <c r="E20">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2.2991738004471007</v>
       </c>
@@ -762,8 +841,12 @@
       <c r="E21">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2.6067385473124975</v>
       </c>
@@ -779,8 +862,12 @@
       <c r="E22">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2.955446801248121</v>
       </c>
@@ -796,8 +883,12 @@
       <c r="E23">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>3.3508024055627086</v>
       </c>
@@ -813,8 +904,12 @@
       <c r="E24">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3.7990454629002808</v>
       </c>
@@ -830,8 +925,12 @@
       <c r="E25">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>4.3072508260180387</v>
       </c>
@@ -847,8 +946,12 @@
       <c r="E26">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>4.8834397638584059</v>
       </c>
@@ -864,8 +967,12 @@
       <c r="E27">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>5.5367065653987897</v>
       </c>
@@ -881,8 +988,12 @@
       <c r="E28">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>6.2773620795333471</v>
       </c>
@@ -898,8 +1009,12 @@
       <c r="E29">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>7.1170964565511561</v>
       </c>
@@ -915,8 +1030,12 @@
       <c r="E30">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>8.0691636598439658</v>
       </c>
@@ -932,8 +1051,12 @@
       <c r="E31">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>9.1485906600876028</v>
       </c>
@@ -949,8 +1072,12 @@
       <c r="E32">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>10.372414613717293</v>
       </c>
@@ -966,8 +1093,12 @@
       <c r="E33">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>11.759951769207897</v>
       </c>
@@ -983,8 +1114,12 @@
       <c r="E34">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>13.333102345446351</v>
       </c>
@@ -1000,8 +1135,12 @@
       <c r="E35">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>15.116696194249871</v>
       </c>
@@ -1017,8 +1156,12 @@
       <c r="E36">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>17.138884702800823</v>
       </c>
@@ -1034,8 +1177,12 @@
       <c r="E37">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>19.431585121597816</v>
       </c>
@@ -1051,8 +1198,12 @@
       <c r="E38">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>22.030984330981411</v>
       </c>
@@ -1068,8 +1219,12 @@
       <c r="E39">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>24.978109997443049</v>
       </c>
@@ -1085,8 +1240,12 @@
       <c r="E40">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>28.319478134573725</v>
       </c>
@@ -1102,8 +1261,12 @@
       <c r="E41">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>32.107827289442561</v>
       </c>
@@ -1119,8 +1282,12 @@
       <c r="E42">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>36.402950942449955</v>
       </c>
@@ -1136,8 +1303,12 @@
       <c r="E43">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>41.272641258854435</v>
       </c>
@@ -1153,8 +1324,12 @@
       <c r="E44">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>46.7937590876925</v>
       </c>
@@ -1170,8 +1345,12 @@
       <c r="E45">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>53.053447096440578</v>
       </c>
@@ -1187,8 +1366,12 @@
       <c r="E46">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>60.150505188952131</v>
       </c>
@@ -1204,8 +1387,12 @@
       <c r="E47">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>68.19694991560489</v>
       </c>
@@ -1221,8 +1408,12 @@
       <c r="E48">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>77.31978248863885</v>
       </c>
@@ -1238,8 +1429,12 @@
       <c r="E49">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>87.662993308186813</v>
       </c>
@@ -1255,8 +1450,12 @@
       <c r="E50">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>99.389834637473129</v>
       </c>
@@ -1272,8 +1471,12 @@
       <c r="E51">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>112.6853972979923</v>
       </c>
@@ -1289,8 +1492,12 @@
       <c r="E52">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>127.75953205398332</v>
       </c>
@@ -1306,8 +1513,12 @@
       <c r="E53">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>144.85016179592955</v>
       </c>
@@ -1323,8 +1534,12 @@
       <c r="E54">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>164.22703680099164</v>
       </c>
@@ -1340,8 +1555,12 @@
       <c r="E55">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>186.19599234159875</v>
       </c>
@@ -1357,8 +1576,12 @@
       <c r="E56">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>211.10377584224526</v>
       </c>
@@ -1374,8 +1597,12 @@
       <c r="E57">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>239.34351977401059</v>
       </c>
@@ -1391,8 +1618,12 @@
       <c r="E58">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>271.36094666833736</v>
       </c>
@@ -1408,8 +1639,12 @@
       <c r="E59">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>307.66140418702167</v>
       </c>
@@ -1425,8 +1660,12 @@
       <c r="E60">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>348.81784128657125</v>
       </c>
@@ -1442,8 +1681,12 @@
       <c r="E61">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>395.47985136887803</v>
       </c>
@@ -1459,8 +1702,12 @@
       <c r="E62">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>448.38392515093909</v>
       </c>
@@ -1476,8 +1723,12 @@
       <c r="E63">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>508.36507507998903</v>
       </c>
@@ -1493,8 +1744,12 @@
       <c r="E64">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>576.3700147682282</v>
       </c>
@@ -1510,8 +1765,12 @@
       <c r="E65">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>653.47210146499015</v>
       </c>
@@ -1527,8 +1786,12 @@
       <c r="E66">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>740.8882774111463</v>
       </c>
@@ -1544,8 +1807,12 @@
       <c r="E67">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <f t="shared" ref="F67:F102" si="1">ROW(F67) - 1</f>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>839.99827746994492</v>
       </c>
@@ -1561,8 +1828,12 @@
       <c r="E68">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <f t="shared" si="1"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>952.3664061982621</v>
       </c>
@@ -1578,8 +1849,12 @@
       <c r="E69">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F69">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>1079.7662280771092</v>
       </c>
@@ -1595,8 +1870,12 @@
       <c r="E70">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F70">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>1224.2085606001081</v>
       </c>
@@ -1612,8 +1891,12 @@
       <c r="E71">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F71">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1387.9732120493375</v>
       </c>
@@ -1629,8 +1912,12 @@
       <c r="E72">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F72">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1573.6449648924213</v>
       </c>
@@ -1646,8 +1933,12 @@
       <c r="E73">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F73">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1784.1543727453727</v>
       </c>
@@ -1663,8 +1954,12 @@
       <c r="E74">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F74">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2022.8240148209368</v>
       </c>
@@ -1680,8 +1975,12 @@
       <c r="E75">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F75">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2293.4209379202975</v>
       </c>
@@ -1697,8 +1996,12 @@
       <c r="E76">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F76">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2600.2161136873892</v>
       </c>
@@ -1714,8 +2017,12 @@
       <c r="E77">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F77">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2948.0518495704537</v>
       </c>
@@ -1731,8 +2038,12 @@
       <c r="E78">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F78">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>3342.4182174730818</v>
       </c>
@@ -1748,8 +2059,12 @@
       <c r="E79">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F79">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>3789.5397064077069</v>
       </c>
@@ -1765,8 +2080,12 @@
       <c r="E80">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F80">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>4296.4734668354795</v>
       </c>
@@ -1782,8 +2101,12 @@
       <c r="E81">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F81">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>4871.2206973337588</v>
       </c>
@@ -1799,8 +2122,12 @@
       <c r="E82">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F82">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>5522.852931664881</v>
       </c>
@@ -1816,8 +2143,12 @@
       <c r="E83">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F83">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>6261.6552195006298</v>
       </c>
@@ -1833,8 +2164,12 @@
       <c r="E84">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F84">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>7099.2884606977823</v>
       </c>
@@ -1850,8 +2185,12 @@
       <c r="E85">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F85">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>8048.9734553312246</v>
       </c>
@@ -1867,8 +2206,12 @@
       <c r="E86">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F86">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>9125.6995744414253</v>
       </c>
@@ -1884,8 +2227,12 @@
       <c r="E87">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F87">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>10346.461345055244</v>
       </c>
@@ -1901,8 +2248,12 @@
       <c r="E88">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F88">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>11730.526683624135</v>
       </c>
@@ -1918,8 +2269,12 @@
       <c r="E89">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F89">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>13299.741011547087</v>
       </c>
@@ -1935,8 +2290,12 @@
       <c r="E90">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F90">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>15078.872052791694</v>
       </c>
@@ -1952,8 +2311,12 @@
       <c r="E91">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F91">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>17096.00075573305</v>
       </c>
@@ -1969,8 +2332,12 @@
       <c r="E92">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F92">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>19382.964509332392</v>
       </c>
@@ -1986,8 +2353,12 @@
       <c r="E93">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F93">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>21975.859649166727</v>
       </c>
@@ -2003,8 +2374,12 @@
       <c r="E94">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F94">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>24915.611184623122</v>
       </c>
@@ -2020,8 +2395,12 @@
       <c r="E95">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F95">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>28248.618739556547</v>
       </c>
@@ -2037,8 +2416,12 @@
       <c r="E96">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F96">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>32027.488901629247</v>
       </c>
@@ -2054,8 +2437,12 @@
       <c r="E97">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F97">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>36311.865539379905</v>
       </c>
@@ -2071,8 +2458,12 @@
       <c r="E98">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F98">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>41169.371192348721</v>
       </c>
@@ -2088,8 +2479,12 @@
       <c r="E99">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F99">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>46676.674392707049</v>
       </c>
@@ -2105,8 +2500,12 @@
       <c r="E100">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F100">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>52920.699764481753</v>
       </c>
@@ -2122,8 +2521,12 @@
       <c r="E101">
         <v>12.521185206834646</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F101">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>60000</v>
       </c>
@@ -2138,6 +2541,10 @@
       </c>
       <c r="E102">
         <v>12.521185206834646</v>
+      </c>
+      <c r="F102">
+        <f t="shared" si="1"/>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -2146,7 +2553,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B0744DC-12F3-409B-B41E-6BE07F633A31}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2158,7 +2565,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF08437C-25BC-4D90-B61E-2EBB7686B57A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>